<commit_message>
Spinks - Typo Fix
</commit_message>
<xml_diff>
--- a/Documents/Archery Madness - Asset List - Primary.xlsx
+++ b/Documents/Archery Madness - Asset List - Primary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Archery_Madness\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D39A851-4D44-4380-871C-CCA0816E3A2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BA64FB-B0A7-46A6-B59F-D9FDD4B1574B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,11 +107,6 @@
     <t>Pirority</t>
   </si>
   <si>
-    <t>The barker is a half wooden mechanized animatronic that is bolted to the bench of the attraction stand. &lt;insert face stuff&gt;. He has a striped tunic red and white tunic. His two arms are whole and functional. His hands are a full flat hand/no fingers with a single unjointed thumb. He is weather worn with peeling paint revealing the wood underneath.
-This hat sits upon the Barkers' head. It is old and weather worn like the barker himself. The paint is old and flaking.
-This wooden bow tie is painted white with purple trimmings and small purple dots. It is weather worn and the paint is flaking.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> -Idle.
  -Two hands pointing right.
  -talking
@@ -127,6 +122,11 @@
     <t xml:space="preserve"> -This but better
  -The quivers will be sticking out of the table.
  -See quiver textures below.</t>
+  </si>
+  <si>
+    <t>The barker is a half wooden mechanized animatronic that is bolted to the bench of the attraction stand. &lt;insert face stuff&gt;. He has a striped tunic red and white tunic. His two arms are whole and functional. His hands are a full flat hand/no fingers with a single unjointed thumb. He is weather worn with peeling paint revealing the wood underneath.
+This hat sits upon the Barkers' head. It is old and weather worn like the barker himself. The paint is old and flaking.
+This wooden bow tie is painted blue. It is weather worn and the paint is flaking.</t>
   </si>
 </sst>
 </file>
@@ -461,7 +461,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6753225" y="2200276"/>
+          <a:off x="7524750" y="304801"/>
           <a:ext cx="1400175" cy="984002"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1182,8 +1182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,10 +1289,10 @@
         <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1357,10 +1357,10 @@
         <v>13</v>
       </c>
       <c r="E13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>